<commit_message>
refactor: Update AssistsController.php to use POST method for sn-schedules report
</commit_message>
<xml_diff>
--- a/public/templates/assists-sn-schedules.xlsx
+++ b/public/templates/assists-sn-schedules.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daust\projects\eda\public\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A85546CD-CB42-491E-9BC1-E6F6E6C2F839}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AA1B1F4-EFFB-44C6-BB44-0BC383B2C083}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{EF595308-AD4D-4EE2-AEBB-2D431F6BA762}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{EF595308-AD4D-4EE2-AEBB-2D431F6BA762}"/>
   </bookViews>
   <sheets>
     <sheet name="Asistencias" sheetId="1" r:id="rId1"/>
@@ -72,7 +72,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -130,14 +130,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="14" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -149,6 +146,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -487,61 +496,65 @@
   <dimension ref="A3:K4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="3" width="9" style="5"/>
-    <col min="4" max="4" width="22.375" customWidth="1"/>
-    <col min="9" max="9" width="13.125" customWidth="1"/>
-    <col min="10" max="10" width="17.25" customWidth="1"/>
-    <col min="11" max="11" width="21.5" customWidth="1"/>
+    <col min="2" max="2" width="9" style="4"/>
+    <col min="3" max="3" width="16.42578125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="6"/>
+    <col min="5" max="5" width="22.42578125" style="6" customWidth="1"/>
+    <col min="6" max="7" width="9.140625" style="6"/>
+    <col min="8" max="8" width="9.140625" style="8"/>
+    <col min="9" max="9" width="9.140625" style="6"/>
+    <col min="10" max="10" width="17.28515625" style="8" customWidth="1"/>
+    <col min="11" max="11" width="21.42578125" style="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:11" ht="81" customHeight="1">
-      <c r="A3" s="5"/>
-      <c r="B3" s="4" t="s">
+    <row r="3" spans="1:11" ht="81" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="4"/>
+      <c r="B3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="E3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="F3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="G3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="H3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="I3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="J3" s="4" t="s">
+      <c r="J3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="K3" s="4" t="s">
+      <c r="K3" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="7"/>
       <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
+      <c r="J4" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>